<commit_message>
added XDJ-XZ and partymix v0.8.1 maps.
</commit_message>
<xml_diff>
--- a/traktor/mapping_party_mix/Source files/PartyMix Mapping - Detailed reference.xlsx
+++ b/traktor/mapping_party_mix/Source files/PartyMix Mapping - Detailed reference.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
   <si>
     <t>Main Function</t>
   </si>
@@ -55,24 +55,12 @@
     <t>Play/Pause</t>
   </si>
   <si>
-    <t>Goto Back</t>
-  </si>
-  <si>
     <t>Cue</t>
   </si>
   <si>
     <t>Bass</t>
   </si>
   <si>
-    <t>Echo depth #2</t>
-  </si>
-  <si>
-    <t>Echo Depth #1</t>
-  </si>
-  <si>
-    <t>FX Depth</t>
-  </si>
-  <si>
     <t>Treble+Mid</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t>Filter</t>
   </si>
   <si>
-    <t>Filter Off</t>
-  </si>
-  <si>
     <t>BROWSE</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>HotCues</t>
-  </si>
-  <si>
     <t>+Scratch</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>Next PadPage</t>
   </si>
   <si>
-    <t>Goto Pad Index</t>
-  </si>
-  <si>
     <t>JOG</t>
   </si>
   <si>
@@ -184,9 +163,6 @@
     <t>LoopRoll</t>
   </si>
   <si>
-    <t>Slip reverse</t>
-  </si>
-  <si>
     <t>FX1 on</t>
   </si>
   <si>
@@ -196,30 +172,9 @@
     <t>Next FX</t>
   </si>
   <si>
-    <t>Goto Cues page</t>
-  </si>
-  <si>
-    <t>BeatJump</t>
-  </si>
-  <si>
-    <t>Slicer</t>
-  </si>
-  <si>
     <t>Loop Roll</t>
   </si>
   <si>
-    <t>KeyCue</t>
-  </si>
-  <si>
-    <t>Loop</t>
-  </si>
-  <si>
-    <t>FX mode</t>
-  </si>
-  <si>
-    <t>PAD INDEX MODE</t>
-  </si>
-  <si>
     <t>LOOP MODE</t>
   </si>
   <si>
@@ -262,10 +217,91 @@
     <t>Sync</t>
   </si>
   <si>
-    <t>FX Grid ++</t>
-  </si>
-  <si>
-    <t>FX Grid --</t>
+    <t>Pad Param ++</t>
+  </si>
+  <si>
+    <t>Pad Param --</t>
+  </si>
+  <si>
+    <t>Go to Beginning</t>
+  </si>
+  <si>
+    <t>CUE PAD MODE</t>
+  </si>
+  <si>
+    <t>Cue 1</t>
+  </si>
+  <si>
+    <t>Cue 2</t>
+  </si>
+  <si>
+    <t>Cue 4</t>
+  </si>
+  <si>
+    <t>Cue 3</t>
+  </si>
+  <si>
+    <t>Delete Cue 1</t>
+  </si>
+  <si>
+    <t>Delete Cue 4</t>
+  </si>
+  <si>
+    <t>Delete Cue 3</t>
+  </si>
+  <si>
+    <t>Delete Cue 2</t>
+  </si>
+  <si>
+    <t>Goto ColorFX</t>
+  </si>
+  <si>
+    <t>Select 4x Pages</t>
+  </si>
+  <si>
+    <t>Bend</t>
+  </si>
+  <si>
+    <t>COLORFX MODE</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Spiral</t>
+  </si>
+  <si>
+    <t>Censor</t>
+  </si>
+  <si>
+    <t>FX parameter #1</t>
+  </si>
+  <si>
+    <t>FX paarmeter #2</t>
+  </si>
+  <si>
+    <t>SAMPLER MODE</t>
+  </si>
+  <si>
+    <t>Air Horn</t>
+  </si>
+  <si>
+    <t>Siren</t>
+  </si>
+  <si>
+    <t>Explosion</t>
+  </si>
+  <si>
+    <t>Applause</t>
+  </si>
+  <si>
+    <t>Laugh</t>
   </si>
 </sst>
 </file>
@@ -275,7 +311,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +366,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -337,8 +380,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FFFFFFFF"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -434,7 +485,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -475,14 +526,29 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -790,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AMJ46"/>
+  <dimension ref="B2:AMJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E46" sqref="B27:E46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -820,23 +886,23 @@
     </row>
     <row r="4" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="9"/>
@@ -846,7 +912,7 @@
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="9"/>
@@ -854,7 +920,7 @@
     </row>
     <row r="7" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
@@ -862,45 +928,43 @@
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="C8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
+      <c r="C9" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>15</v>
+      <c r="C10" s="19" t="s">
+        <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
     </row>
@@ -908,33 +972,33 @@
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>60</v>
+      <c r="C12" s="19" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>42</v>
+      <c r="C13" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
@@ -942,11 +1006,11 @@
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>81</v>
+      <c r="C15" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -954,11 +1018,11 @@
       <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>14</v>
+      <c r="C16" s="19" t="s">
+        <v>13</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -966,294 +1030,447 @@
       <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="10"/>
+        <v>33</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="D22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="26" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="E26" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="6" t="s">
+      <c r="D50" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
+      <c r="D54" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+      <c r="D56" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="E56" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>77</v>
-      </c>
+      <c r="E58" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>

</xml_diff>